<commit_message>
planning of iteration 2
</commit_message>
<xml_diff>
--- a/prjplanning/Iteration1.xlsx
+++ b/prjplanning/Iteration1.xlsx
@@ -949,11 +949,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93349376"/>
-        <c:axId val="93350912"/>
+        <c:axId val="94660480"/>
+        <c:axId val="94662016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="93349376"/>
+        <c:axId val="94660480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +973,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93350912"/>
+        <c:crossAx val="94662016"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -984,7 +984,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="93350912"/>
+        <c:axId val="94662016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1016,7 +1016,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93349376"/>
+        <c:crossAx val="94660480"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -1744,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>